<commit_message>
commit prior to edits for library submissions, likely no edits to be made for this
</commit_message>
<xml_diff>
--- a/Data/OK_musical_ensemble_scenes.xlsx
+++ b/Data/OK_musical_ensemble_scenes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mqoutlook-my.sharepoint.com/personal/austin_megier_hdr_mq_edu_au/Documents/MRes_Thesis_Data/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mqoutlook-my.sharepoint.com/personal/austin_megier_hdr_mq_edu_au/Documents/MRes/MRes_Thesis_Data/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7345" documentId="8_{54466117-68E5-FA45-A62B-69B7A0496348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D4062C3-7230-3C4E-8656-DE2A249D7762}"/>
+  <xr:revisionPtr revIDLastSave="7349" documentId="8_{54466117-68E5-FA45-A62B-69B7A0496348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3E64C46-4B56-0A4E-9446-95329682A08B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" activeTab="3" xr2:uid="{F188212D-6757-6E45-81FC-2E36196F77A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="2" xr2:uid="{F188212D-6757-6E45-81FC-2E36196F77A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4406" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="771">
   <si>
     <t>Room</t>
   </si>
@@ -2357,6 +2357,9 @@
   </si>
   <si>
     <t>Ptahhotep Iyniankh</t>
+  </si>
+  <si>
+    <t>NK</t>
   </si>
 </sst>
 </file>
@@ -4847,7 +4850,7 @@
   <dimension ref="A1:I259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -15743,7 +15746,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15958,7 +15961,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -21371,17 +21374,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D8B279-056F-1F4B-95AB-FEAD2B0ED30A}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>611</v>
       </c>
       <c r="B1" t="s">
@@ -22156,6 +22159,17 @@
       </c>
       <c r="C35" t="s">
         <v>96</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="B36" t="s">
+        <v>770</v>
       </c>
     </row>
   </sheetData>
@@ -22167,9 +22181,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00059BFA-7364-4145-88BE-C4AB55199DE3}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -23483,7 +23497,7 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -24398,7 +24412,7 @@
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
@@ -26196,7 +26210,7 @@
   <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C232" sqref="C232"/>
     </sheetView>
   </sheetViews>

</xml_diff>